<commit_message>
Update Planilha Análise Cohort Retenção de Clientes Compras.xlsx
</commit_message>
<xml_diff>
--- a/Projetos/Projeto 02 - Análise Cohort Com Excel/Planilha Análise Cohort Retenção de Clientes Compras.xlsx
+++ b/Projetos/Projeto 02 - Análise Cohort Com Excel/Planilha Análise Cohort Retenção de Clientes Compras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edutr\OneDrive\Documentos\Portifólio\GitHub\Analise_Dados\Projetos\Projeto 02 - Análise Cohort Com Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C122DB34-3F19-405B-A36F-0998EFE438CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224627BD-56AF-4505-B25E-DA1F6F973D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11706412-9C5A-4854-89B5-859A677D4F19}"/>
   </bookViews>
@@ -92,13 +92,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>132708</xdr:rowOff>
+      <xdr:rowOff>132709</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>91439</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>178843</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -128,8 +128,69 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="213360" y="132708"/>
-          <a:ext cx="8808720" cy="4347851"/>
+          <a:off x="213360" y="132709"/>
+          <a:ext cx="5280660" cy="2606454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>105613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2" descr="Análise Cohort: como fazer e por que é importante para PMs">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBE91538-6D51-4404-8459-81AF44427535}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5798820" y="297180"/>
+          <a:ext cx="6637020" cy="4380433"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -471,7 +532,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>